<commit_message>
states, graphs and something else, i don't remember
</commit_message>
<xml_diff>
--- a/app/src/main/res/raw/dot.xlsx
+++ b/app/src/main/res/raw/dot.xlsx
@@ -287,22 +287,22 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <xdr:twoCellAnchor editAs="absolute">
+  <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>172800</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>47160</xdr:rowOff>
+      <xdr:rowOff>12240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>846000</xdr:colOff>
+      <xdr:colOff>897120</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>20880</xdr:rowOff>
+      <xdr:rowOff>166680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="Изображение 1" descr=""/>
+        <xdr:cNvPr id="0" name="Изображение 2" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -311,8 +311,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7388640" y="47160"/>
-          <a:ext cx="673200" cy="716400"/>
+          <a:off x="7215840" y="12240"/>
+          <a:ext cx="897120" cy="897120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -335,10 +335,10 @@
   <dimension ref="A1:F47"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G20" activeCellId="0" sqref="G20"/>
+      <selection pane="topLeft" activeCell="I14" activeCellId="0" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="1" style="0" width="25.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.57"/>

</xml_diff>